<commit_message>
Done with feedack changes
</commit_message>
<xml_diff>
--- a/TestData/allInOne.xlsx
+++ b/TestData/allInOne.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pranav Pawar\PycharmProjects\RMM_DataDriven\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{679A693F-789F-4FCE-8285-1B211D22F8DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F85AE5A-72C5-4FFB-B53A-9C438955159B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2808" yWindow="1932" windowWidth="16236" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="62">
   <si>
     <t>Operation</t>
   </si>
@@ -208,6 +208,9 @@
   </si>
   <si>
     <t>./TestData/firstFlow/addPolicyToWave.xlsx</t>
+  </si>
+  <si>
+    <t>Cloud / vCenter Name</t>
   </si>
 </sst>
 </file>
@@ -554,27 +557,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J33"/>
+  <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="24" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="49.77734375" customWidth="1"/>
+    <col min="2" max="2" width="77.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20" customWidth="1"/>
-    <col min="5" max="5" width="11.109375" customWidth="1"/>
-    <col min="6" max="6" width="21.5546875" customWidth="1"/>
-    <col min="7" max="7" width="13.44140625" customWidth="1"/>
+    <col min="4" max="4" width="20.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.44140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.44140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -605,8 +609,11 @@
       <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K1" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -617,7 +624,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -625,7 +632,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -633,7 +640,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -644,7 +651,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -652,7 +659,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -666,7 +673,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -680,7 +687,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -694,7 +701,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>25</v>
       </c>
@@ -702,7 +709,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -710,7 +717,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>29</v>
       </c>
@@ -721,7 +728,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>29</v>
       </c>
@@ -732,7 +739,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>32</v>
       </c>
@@ -740,7 +747,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>33</v>
       </c>
@@ -748,7 +755,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>35</v>
       </c>

</xml_diff>